<commit_message>
changed excel spreadsheet and added concept document
</commit_message>
<xml_diff>
--- a/your game name here.xlsx
+++ b/your game name here.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter.lowe\Desktop\proto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/505adff6d4132b90/Desktop/Concept Doc/concept25-Nicholas-McDonald-05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592968BF-B044-48C7-B482-7309AED76571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{592968BF-B044-48C7-B482-7309AED76571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E45844D-24AF-436C-82C8-A6B20FCC947D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B114BF61-C9F1-47F8-B51B-C5362F104DFD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B114BF61-C9F1-47F8-B51B-C5362F104DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
-    <t xml:space="preserve">Your Game Name Here </t>
-  </si>
-  <si>
     <t>want 20-30% each</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Check that yellow boxes are reasonably even</t>
+  </si>
+  <si>
+    <t>Going Up!</t>
   </si>
 </sst>
 </file>
@@ -311,9 +311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -351,7 +351,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -457,7 +457,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -599,7 +599,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -610,21 +610,21 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="11" width="4.28515625" customWidth="1"/>
-    <col min="14" max="17" width="3.85546875" customWidth="1"/>
+    <col min="1" max="2" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="11" width="4.33203125" customWidth="1"/>
+    <col min="14" max="17" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1"/>
       <c r="N1" s="10">
@@ -644,10 +644,10 @@
         <v>0</v>
       </c>
       <c r="S1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C2">
         <f>SUM(C4:C23)</f>
         <v>50</v>
@@ -658,51 +658,51 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(G4:G23)</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
-        <v>5</v>
-      </c>
       <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>8</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" t="s">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="str">
@@ -710,15 +710,15 @@
         <v>Value</v>
       </c>
       <c r="N3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -762,17 +762,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6">
+        <v>15</v>
+      </c>
       <c r="E5">
         <v>25</v>
       </c>
@@ -782,7 +784,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -809,17 +811,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
       <c r="E6">
         <v>5</v>
       </c>
@@ -829,7 +833,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -856,17 +860,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <v>10</v>
+      </c>
       <c r="E7">
         <v>15</v>
       </c>
@@ -876,7 +882,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -903,17 +909,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6">
+        <v>5</v>
+      </c>
       <c r="E8">
         <v>15</v>
       </c>
@@ -923,7 +931,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -950,12 +958,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -999,12 +1007,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -1048,17 +1056,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
       <c r="E11">
         <v>20</v>
       </c>
@@ -1068,7 +1078,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -1095,12 +1105,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1144,17 +1154,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="6">
+        <v>10</v>
+      </c>
       <c r="E13">
         <v>20</v>
       </c>
@@ -1164,7 +1176,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1191,58 +1203,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="4" t="s">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>